<commit_message>
Definition of the data types
Valid Data Types
values must be one of the following data types:

a string
a number
null
</commit_message>
<xml_diff>
--- a/Documentation.xlsx
+++ b/Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinzimmermann/nexio/3_R&amp;D/Projet Haag-Streit Phoroptère/GitHub/refractive-JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC513B5B-8A4F-9E4A-8766-9B6E285CB214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECBB1F3-7131-F843-AB39-D249E2113BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26880" xr2:uid="{97470A89-5A9D-474B-83A0-7CF02DF1D5C9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="230">
   <si>
     <t>{</t>
   </si>
@@ -555,6 +555,9 @@
   </si>
   <si>
     <t>Vertical prism power ( △ )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spherical equivalent value </t>
   </si>
   <si>
     <r>
@@ -740,9 +743,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Defines the output path of the json,if data is provided in a transmitted json (LM, AR, CO) it will be overwritten  the phoropter settings</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fixed value (JSON is always in dioptres) </t>
   </si>
   <si>
@@ -807,6 +807,9 @@
   </si>
   <si>
     <t>Vertex distance unit (fixed value)</t>
+  </si>
+  <si>
+    <t>Defines the output path of the json,if data is provided in a transmitted json (LM, AR, CO) it will be overwritten the phoropter settings</t>
   </si>
 </sst>
 </file>
@@ -1277,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CFF79E-0D8B-AF4F-8800-07737C044728}">
   <dimension ref="A1:Q389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A306" zoomScale="139" workbookViewId="0">
-      <selection activeCell="M329" sqref="M329"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="139" workbookViewId="0">
+      <selection activeCell="J131" sqref="J131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1"/>
@@ -1316,7 +1319,7 @@
         <v>82</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1405,7 +1408,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>88</v>
@@ -1414,7 +1417,7 @@
         <v>84</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="34">
@@ -1422,7 +1425,7 @@
         <v>7</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>88</v>
@@ -1431,10 +1434,10 @@
         <v>84</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1476,7 +1479,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="E16" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>91</v>
@@ -1616,7 +1619,7 @@
         <v>89</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="5:12">
@@ -1642,7 +1645,7 @@
         <v>101</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>89</v>
@@ -1665,7 +1668,7 @@
         <v>89</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="5:12">
@@ -1744,7 +1747,7 @@
         <v>107</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>89</v>
@@ -1758,7 +1761,7 @@
         <v>27</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>88</v>
@@ -1791,7 +1794,7 @@
         <v>109</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>89</v>
@@ -1837,7 +1840,7 @@
         <v>32</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>88</v>
@@ -1866,7 +1869,7 @@
         <v>111</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="4:13">
@@ -1879,7 +1882,7 @@
         <v>32</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>88</v>
@@ -1902,7 +1905,7 @@
         <v>115</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>111</v>
@@ -2055,7 +2058,7 @@
         <v>89</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="5:13">
@@ -2092,7 +2095,7 @@
         <v>89</v>
       </c>
       <c r="L57" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="5:13">
@@ -2109,7 +2112,7 @@
         <v>89</v>
       </c>
       <c r="L58" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="5:13">
@@ -2126,7 +2129,7 @@
         <v>89</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="5:13">
@@ -2143,7 +2146,7 @@
         <v>89</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="61" spans="5:13">
@@ -2250,7 +2253,7 @@
         <v>111</v>
       </c>
       <c r="L67" s="17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M67" s="1" t="s">
         <v>212</v>
@@ -2476,7 +2479,7 @@
         <v>89</v>
       </c>
       <c r="L88" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M88" s="1" t="s">
         <v>216</v>
@@ -2625,7 +2628,7 @@
         <v>32</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J117" s="2" t="s">
         <v>88</v>
@@ -2654,7 +2657,7 @@
         <v>111</v>
       </c>
       <c r="L118" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="119" spans="4:13">
@@ -2667,7 +2670,7 @@
         <v>32</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J120" s="2" t="s">
         <v>88</v>
@@ -2690,7 +2693,7 @@
         <v>115</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K121" s="5" t="s">
         <v>111</v>
@@ -2756,7 +2759,7 @@
         <v>111</v>
       </c>
       <c r="L125" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M125" s="19"/>
     </row>
@@ -2775,22 +2778,24 @@
         <v>41</v>
       </c>
       <c r="I128" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="K128" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="L128" s="2"/>
+      <c r="L128" s="12" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="129" spans="6:12">
       <c r="G129" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I129" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J129" s="2" t="s">
         <v>20</v>
@@ -2799,7 +2804,7 @@
         <v>89</v>
       </c>
       <c r="L129" s="12" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="130" spans="6:12">
@@ -2807,7 +2812,7 @@
         <v>43</v>
       </c>
       <c r="I130" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J130" s="2" t="s">
         <v>20</v>
@@ -2816,7 +2821,7 @@
         <v>89</v>
       </c>
       <c r="L130" s="12" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="131" spans="6:12">
@@ -2824,16 +2829,16 @@
         <v>60</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>126</v>
+        <v>168</v>
       </c>
       <c r="J131" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K131" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L131" s="12" t="s">
-        <v>201</v>
+      <c r="K131" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="L131" s="6">
+        <v>-3.5</v>
       </c>
     </row>
     <row r="132" spans="6:12">
@@ -2906,7 +2911,7 @@
     </row>
     <row r="136" spans="6:12">
       <c r="G136" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I136" s="13"/>
       <c r="J136" s="13"/>
@@ -2935,19 +2940,19 @@
         <v>69</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J138" s="8"/>
       <c r="K138" s="5" t="s">
         <v>111</v>
       </c>
       <c r="L138" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="139" spans="6:12">
       <c r="G139" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I139" s="13"/>
       <c r="J139" s="13"/>
@@ -2985,7 +2990,7 @@
         <v>111</v>
       </c>
       <c r="L141" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="142" spans="6:12">
@@ -3295,7 +3300,7 @@
         <v>32</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J192" s="2" t="s">
         <v>88</v>
@@ -3324,7 +3329,7 @@
         <v>111</v>
       </c>
       <c r="L193" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="194" spans="6:13">
@@ -3337,7 +3342,7 @@
         <v>32</v>
       </c>
       <c r="I195" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J195" s="2" t="s">
         <v>88</v>
@@ -3360,7 +3365,7 @@
         <v>115</v>
       </c>
       <c r="J196" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K196" s="5" t="s">
         <v>111</v>
@@ -3516,7 +3521,7 @@
         <v>111</v>
       </c>
       <c r="L206" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M206" s="19"/>
     </row>
@@ -3574,7 +3579,7 @@
         <v>89</v>
       </c>
       <c r="L210" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="211" spans="5:12">
@@ -3611,7 +3616,7 @@
         <v>89</v>
       </c>
       <c r="L213" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="214" spans="5:12">
@@ -3628,7 +3633,7 @@
         <v>89</v>
       </c>
       <c r="L214" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="215" spans="5:12">
@@ -3645,7 +3650,7 @@
         <v>89</v>
       </c>
       <c r="L215" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="216" spans="5:12">
@@ -3718,7 +3723,7 @@
     </row>
     <row r="220" spans="5:12">
       <c r="G220" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I220" s="13"/>
       <c r="J220" s="13"/>
@@ -3747,19 +3752,19 @@
         <v>69</v>
       </c>
       <c r="I222" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J222" s="8"/>
       <c r="K222" s="5" t="s">
         <v>111</v>
       </c>
       <c r="L222" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="223" spans="5:12">
       <c r="G223" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I223" s="13"/>
       <c r="J223" s="13"/>
@@ -3797,7 +3802,7 @@
         <v>111</v>
       </c>
       <c r="L225" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="226" spans="6:13">
@@ -3814,7 +3819,7 @@
         <v>89</v>
       </c>
       <c r="L226" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="227" spans="6:13">
@@ -3921,7 +3926,7 @@
         <v>111</v>
       </c>
       <c r="L233" s="17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M233" s="1" t="s">
         <v>212</v>
@@ -4074,7 +4079,7 @@
     </row>
     <row r="259" spans="6:12">
       <c r="G259" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I259" s="2"/>
       <c r="J259" s="2"/>
@@ -4083,56 +4088,56 @@
     </row>
     <row r="260" spans="6:12">
       <c r="H260" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I260" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J260" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K260" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L260" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="261" spans="6:12">
       <c r="H261" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I261" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J261" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K261" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L261" s="2"/>
     </row>
     <row r="262" spans="6:12">
       <c r="H262" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I262" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J262" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K262" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L262" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="263" spans="6:12">
       <c r="G263" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I263" s="2"/>
       <c r="J263" s="2"/>
@@ -4141,51 +4146,51 @@
     </row>
     <row r="264" spans="6:12">
       <c r="H264" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I264" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J264" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K264" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L264" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="265" spans="6:12">
       <c r="H265" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I265" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J265" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K265" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L265" s="2"/>
     </row>
     <row r="266" spans="6:12">
       <c r="H266" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I266" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J266" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K266" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L266" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="267" spans="6:12">
@@ -4193,13 +4198,13 @@
         <v>74</v>
       </c>
       <c r="I267" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J267" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K267" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L267" s="2"/>
     </row>
@@ -4208,13 +4213,13 @@
         <v>75</v>
       </c>
       <c r="I268" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J268" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K268" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L268" s="2"/>
     </row>
@@ -4485,7 +4490,7 @@
         <v>32</v>
       </c>
       <c r="I305" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J305" s="2" t="s">
         <v>88</v>
@@ -4514,7 +4519,7 @@
         <v>111</v>
       </c>
       <c r="L306" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="307" spans="6:13">
@@ -4527,7 +4532,7 @@
         <v>32</v>
       </c>
       <c r="I308" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J308" s="2" t="s">
         <v>88</v>
@@ -4550,7 +4555,7 @@
         <v>115</v>
       </c>
       <c r="J309" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K309" s="5" t="s">
         <v>111</v>
@@ -4706,7 +4711,7 @@
         <v>111</v>
       </c>
       <c r="L319" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M319" s="19"/>
     </row>
@@ -4764,7 +4769,7 @@
         <v>89</v>
       </c>
       <c r="L323" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="324" spans="5:13">
@@ -4801,7 +4806,7 @@
         <v>89</v>
       </c>
       <c r="L326" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="327" spans="5:13">
@@ -4818,7 +4823,7 @@
         <v>89</v>
       </c>
       <c r="L327" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="328" spans="5:13">
@@ -4835,7 +4840,7 @@
         <v>89</v>
       </c>
       <c r="L328" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="329" spans="5:13">
@@ -4908,7 +4913,7 @@
     </row>
     <row r="333" spans="5:13">
       <c r="G333" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I333" s="13"/>
       <c r="J333" s="13"/>
@@ -4937,19 +4942,19 @@
         <v>69</v>
       </c>
       <c r="I335" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J335" s="8"/>
       <c r="K335" s="5" t="s">
         <v>111</v>
       </c>
       <c r="L335" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="336" spans="5:13">
       <c r="G336" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I336" s="13"/>
       <c r="J336" s="13"/>
@@ -4987,7 +4992,7 @@
         <v>111</v>
       </c>
       <c r="L338" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="339" spans="6:13">
@@ -5004,7 +5009,7 @@
         <v>89</v>
       </c>
       <c r="L339" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="340" spans="6:13">
@@ -5111,7 +5116,7 @@
         <v>111</v>
       </c>
       <c r="L346" s="17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M346" s="1" t="s">
         <v>212</v>
@@ -5264,7 +5269,7 @@
     </row>
     <row r="372" spans="6:12">
       <c r="G372" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I372" s="2"/>
       <c r="J372" s="2"/>
@@ -5273,56 +5278,56 @@
     </row>
     <row r="373" spans="6:12">
       <c r="H373" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I373" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J373" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K373" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L373" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="374" spans="6:12">
       <c r="H374" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I374" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J374" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K374" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L374" s="2"/>
     </row>
     <row r="375" spans="6:12">
       <c r="H375" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I375" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J375" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K375" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L375" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="376" spans="6:12">
       <c r="G376" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I376" s="2"/>
       <c r="J376" s="2"/>
@@ -5331,51 +5336,51 @@
     </row>
     <row r="377" spans="6:12">
       <c r="H377" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I377" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J377" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K377" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L377" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="378" spans="6:12">
       <c r="H378" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I378" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J378" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K378" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L378" s="2"/>
     </row>
     <row r="379" spans="6:12">
       <c r="H379" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I379" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J379" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K379" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L379" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="380" spans="6:12">
@@ -5383,13 +5388,13 @@
         <v>74</v>
       </c>
       <c r="I380" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J380" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K380" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L380" s="2"/>
     </row>
@@ -5398,13 +5403,13 @@
         <v>75</v>
       </c>
       <c r="I381" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J381" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K381" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L381" s="2"/>
     </row>

</xml_diff>

<commit_message>
Add info for prisms
</commit_message>
<xml_diff>
--- a/Documentation.xlsx
+++ b/Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinzimmermann/Github/refractive-JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558133F0-941E-8145-A688-89575444E15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6733FCAA-8947-4843-8D09-173369FA4428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="41840" windowHeight="23420" xr2:uid="{97470A89-5A9D-474B-83A0-7CF02DF1D5C9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{97470A89-5A9D-474B-83A0-7CF02DF1D5C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="235">
   <si>
     <t>{</t>
   </si>
@@ -659,9 +659,6 @@
     <t>Json end point</t>
   </si>
   <si>
-    <t>in or out</t>
-  </si>
-  <si>
     <t>Snellen, Logarithmic, Decimal</t>
   </si>
   <si>
@@ -677,9 +674,6 @@
     <t>(base Up and base Down only)</t>
   </si>
   <si>
-    <t>up or down</t>
-  </si>
-  <si>
     <t>divergence:{</t>
   </si>
   <si>
@@ -819,6 +813,18 @@
   </si>
   <si>
     <t>allows the filiation of datasets to a unique source for example TonoRef III AR, TONO, PACHY,…</t>
+  </si>
+  <si>
+    <t>U or D</t>
+  </si>
+  <si>
+    <t>I or O</t>
+  </si>
+  <si>
+    <t>This field is mandatory if a Horizontal prism power is entered</t>
+  </si>
+  <si>
+    <t>This field is mandatory if a Vertical prism power is entered</t>
   </si>
 </sst>
 </file>
@@ -1299,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CFF79E-0D8B-AF4F-8800-07737C044728}">
   <dimension ref="A1:Q410"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A321" zoomScale="137" workbookViewId="0">
+      <selection activeCell="M340" sqref="M340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1"/>
@@ -1338,7 +1344,7 @@
         <v>82</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1436,7 +1442,7 @@
         <v>84</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="34">
@@ -1453,10 +1459,10 @@
         <v>84</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1498,7 +1504,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="E16" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>91</v>
@@ -1575,7 +1581,7 @@
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="5:13">
@@ -1641,7 +1647,7 @@
         <v>89</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="5:13">
@@ -1667,7 +1673,7 @@
         <v>101</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>89</v>
@@ -1690,7 +1696,7 @@
         <v>89</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="5:13">
@@ -1769,7 +1775,7 @@
         <v>107</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>89</v>
@@ -1783,7 +1789,7 @@
         <v>27</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>88</v>
@@ -1816,7 +1822,7 @@
         <v>109</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>89</v>
@@ -1862,7 +1868,7 @@
         <v>32</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>88</v>
@@ -1874,7 +1880,7 @@
         <v>112</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="4:13">
@@ -1891,7 +1897,7 @@
         <v>111</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="4:13">
@@ -1904,7 +1910,7 @@
         <v>32</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>88</v>
@@ -1916,7 +1922,7 @@
         <v>114</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="4:13">
@@ -1927,7 +1933,7 @@
         <v>115</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>111</v>
@@ -1963,7 +1969,7 @@
         <v>89</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="4:13">
@@ -2008,7 +2014,7 @@
         <v>89</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="5:13">
@@ -2036,7 +2042,7 @@
         <v>32</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>88</v>
@@ -2048,7 +2054,7 @@
         <v>120</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="5:13">
@@ -2080,7 +2086,7 @@
         <v>89</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="5:13">
@@ -2117,7 +2123,7 @@
         <v>89</v>
       </c>
       <c r="L57" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="58" spans="5:13">
@@ -2134,7 +2140,7 @@
         <v>89</v>
       </c>
       <c r="L58" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="5:13">
@@ -2151,7 +2157,7 @@
         <v>89</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="5:13">
@@ -2168,7 +2174,7 @@
         <v>89</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" spans="5:13">
@@ -2266,7 +2272,7 @@
         <v>51</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>20</v>
@@ -2275,10 +2281,10 @@
         <v>111</v>
       </c>
       <c r="L67" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="68" spans="6:13">
@@ -2472,7 +2478,7 @@
         <v>54</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>20</v>
@@ -2481,10 +2487,10 @@
         <v>111</v>
       </c>
       <c r="L87" s="17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="3:13">
@@ -2501,10 +2507,10 @@
         <v>89</v>
       </c>
       <c r="L88" s="17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="90" spans="3:13">
@@ -2650,7 +2656,7 @@
         <v>32</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J117" s="2" t="s">
         <v>88</v>
@@ -2662,7 +2668,7 @@
         <v>112</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="118" spans="4:13">
@@ -2679,7 +2685,7 @@
         <v>111</v>
       </c>
       <c r="L118" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="119" spans="4:13">
@@ -2692,7 +2698,7 @@
         <v>32</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J120" s="2" t="s">
         <v>88</v>
@@ -2704,7 +2710,7 @@
         <v>114</v>
       </c>
       <c r="M120" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="121" spans="4:13">
@@ -2715,7 +2721,7 @@
         <v>115</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K121" s="5" t="s">
         <v>111</v>
@@ -2746,7 +2752,7 @@
         <v>149</v>
       </c>
       <c r="M123" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="124" spans="4:13">
@@ -2763,7 +2769,7 @@
         <v>111</v>
       </c>
       <c r="L124" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M124" s="23"/>
     </row>
@@ -2781,7 +2787,7 @@
         <v>111</v>
       </c>
       <c r="L125" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M125" s="23"/>
     </row>
@@ -2809,10 +2815,10 @@
         <v>89</v>
       </c>
       <c r="L128" s="12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="129" spans="6:12">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="129" spans="6:13">
       <c r="G129" s="1" t="s">
         <v>42</v>
       </c>
@@ -2826,10 +2832,10 @@
         <v>89</v>
       </c>
       <c r="L129" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="130" spans="6:12">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="130" spans="6:13">
       <c r="G130" s="1" t="s">
         <v>43</v>
       </c>
@@ -2843,10 +2849,10 @@
         <v>89</v>
       </c>
       <c r="L130" s="12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="131" spans="6:12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="131" spans="6:13">
       <c r="G131" s="1" t="s">
         <v>60</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>-3.5</v>
       </c>
     </row>
-    <row r="132" spans="6:12">
+    <row r="132" spans="6:13">
       <c r="G132" s="1" t="s">
         <v>61</v>
       </c>
@@ -2877,10 +2883,10 @@
         <v>111</v>
       </c>
       <c r="L132" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="133" spans="6:12">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="133" spans="6:13">
       <c r="G133" s="1" t="s">
         <v>62</v>
       </c>
@@ -2894,10 +2900,10 @@
         <v>111</v>
       </c>
       <c r="L133" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="134" spans="6:12">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="134" spans="6:13">
       <c r="G134" s="1" t="s">
         <v>63</v>
       </c>
@@ -2911,10 +2917,10 @@
         <v>111</v>
       </c>
       <c r="L134" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="135" spans="6:12">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="135" spans="6:13">
       <c r="G135" s="1" t="s">
         <v>64</v>
       </c>
@@ -2928,19 +2934,19 @@
         <v>111</v>
       </c>
       <c r="L135" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="136" spans="6:12">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="136" spans="6:13">
       <c r="G136" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I136" s="13"/>
       <c r="J136" s="13"/>
       <c r="K136" s="14"/>
       <c r="L136" s="14"/>
     </row>
-    <row r="137" spans="6:12">
+    <row r="137" spans="6:13">
       <c r="H137" s="1" t="s">
         <v>68</v>
       </c>
@@ -2954,34 +2960,37 @@
         <v>111</v>
       </c>
       <c r="L137" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="138" spans="6:12">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="138" spans="6:13">
       <c r="H138" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J138" s="8"/>
       <c r="K138" s="5" t="s">
         <v>111</v>
       </c>
       <c r="L138" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="139" spans="6:12">
+        <v>231</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="139" spans="6:13">
       <c r="G139" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I139" s="13"/>
       <c r="J139" s="13"/>
       <c r="K139" s="14"/>
       <c r="L139" s="14"/>
     </row>
-    <row r="140" spans="6:12">
+    <row r="140" spans="6:13">
       <c r="H140" s="1" t="s">
         <v>68</v>
       </c>
@@ -2995,10 +3004,10 @@
         <v>111</v>
       </c>
       <c r="L140" s="6" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="141" spans="6:12">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="141" spans="6:13">
       <c r="H141" s="1" t="s">
         <v>69</v>
       </c>
@@ -3012,10 +3021,13 @@
         <v>111</v>
       </c>
       <c r="L141" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="142" spans="6:12">
+        <v>232</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="142" spans="6:13">
       <c r="G142" s="1" t="s">
         <v>51</v>
       </c>
@@ -3029,10 +3041,10 @@
         <v>111</v>
       </c>
       <c r="L142" s="17" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="143" spans="6:12">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="143" spans="6:13">
       <c r="F143" s="1" t="s">
         <v>52</v>
       </c>
@@ -3043,7 +3055,7 @@
       <c r="K143" s="14"/>
       <c r="L143" s="14"/>
     </row>
-    <row r="144" spans="6:12" hidden="1" outlineLevel="1">
+    <row r="144" spans="6:13" hidden="1" outlineLevel="1">
       <c r="G144" s="1" t="s">
         <v>41</v>
       </c>
@@ -3159,7 +3171,7 @@
         <v>111</v>
       </c>
       <c r="L162" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="163" spans="3:12">
@@ -3176,7 +3188,7 @@
         <v>111</v>
       </c>
       <c r="L163" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="165" spans="3:12">
@@ -3322,7 +3334,7 @@
         <v>32</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J192" s="2" t="s">
         <v>88</v>
@@ -3334,7 +3346,7 @@
         <v>112</v>
       </c>
       <c r="M192" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="193" spans="6:13">
@@ -3351,7 +3363,7 @@
         <v>111</v>
       </c>
       <c r="L193" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="194" spans="6:13">
@@ -3364,7 +3376,7 @@
         <v>32</v>
       </c>
       <c r="I195" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J195" s="2" t="s">
         <v>88</v>
@@ -3376,7 +3388,7 @@
         <v>114</v>
       </c>
       <c r="M195" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="196" spans="6:13">
@@ -3387,7 +3399,7 @@
         <v>115</v>
       </c>
       <c r="J196" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K196" s="5" t="s">
         <v>111</v>
@@ -3423,7 +3435,7 @@
         <v>89</v>
       </c>
       <c r="L198" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="199" spans="6:13">
@@ -3468,7 +3480,7 @@
         <v>89</v>
       </c>
       <c r="L201" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="202" spans="6:13">
@@ -3508,7 +3520,7 @@
         <v>149</v>
       </c>
       <c r="M204" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="205" spans="6:13">
@@ -3525,7 +3537,7 @@
         <v>111</v>
       </c>
       <c r="L205" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M205" s="23"/>
     </row>
@@ -3543,7 +3555,7 @@
         <v>111</v>
       </c>
       <c r="L206" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M206" s="23"/>
     </row>
@@ -3557,7 +3569,7 @@
         <v>32</v>
       </c>
       <c r="I208" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J208" s="2" t="s">
         <v>88</v>
@@ -3569,10 +3581,10 @@
         <v>120</v>
       </c>
       <c r="M208" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="209" spans="5:12">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="209" spans="5:13">
       <c r="G209" s="1" t="s">
         <v>33</v>
       </c>
@@ -3587,7 +3599,7 @@
       </c>
       <c r="L209" s="2"/>
     </row>
-    <row r="210" spans="5:12">
+    <row r="210" spans="5:13">
       <c r="F210" s="1" t="s">
         <v>38</v>
       </c>
@@ -3601,15 +3613,15 @@
         <v>89</v>
       </c>
       <c r="L210" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="211" spans="5:12">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="211" spans="5:13">
       <c r="E211" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="212" spans="5:12">
+    <row r="212" spans="5:13">
       <c r="F212" s="1" t="s">
         <v>40</v>
       </c>
@@ -3624,7 +3636,7 @@
       </c>
       <c r="L212" s="2"/>
     </row>
-    <row r="213" spans="5:12">
+    <row r="213" spans="5:13">
       <c r="G213" s="1" t="s">
         <v>41</v>
       </c>
@@ -3638,10 +3650,10 @@
         <v>89</v>
       </c>
       <c r="L213" s="12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="214" spans="5:12">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="214" spans="5:13">
       <c r="G214" s="1" t="s">
         <v>42</v>
       </c>
@@ -3655,10 +3667,10 @@
         <v>89</v>
       </c>
       <c r="L214" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="215" spans="5:12">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="215" spans="5:13">
       <c r="G215" s="1" t="s">
         <v>43</v>
       </c>
@@ -3672,10 +3684,10 @@
         <v>89</v>
       </c>
       <c r="L215" s="12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="216" spans="5:12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="216" spans="5:13">
       <c r="G216" s="1" t="s">
         <v>61</v>
       </c>
@@ -3689,10 +3701,10 @@
         <v>111</v>
       </c>
       <c r="L216" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="217" spans="5:12">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="217" spans="5:13">
       <c r="G217" s="1" t="s">
         <v>62</v>
       </c>
@@ -3706,10 +3718,10 @@
         <v>111</v>
       </c>
       <c r="L217" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="218" spans="5:12">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="218" spans="5:13">
       <c r="G218" s="1" t="s">
         <v>63</v>
       </c>
@@ -3723,10 +3735,10 @@
         <v>111</v>
       </c>
       <c r="L218" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="219" spans="5:12">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="219" spans="5:13">
       <c r="G219" s="1" t="s">
         <v>64</v>
       </c>
@@ -3740,19 +3752,19 @@
         <v>111</v>
       </c>
       <c r="L219" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="220" spans="5:12">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="220" spans="5:13">
       <c r="G220" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I220" s="13"/>
       <c r="J220" s="13"/>
       <c r="K220" s="14"/>
       <c r="L220" s="14"/>
     </row>
-    <row r="221" spans="5:12">
+    <row r="221" spans="5:13">
       <c r="H221" s="1" t="s">
         <v>68</v>
       </c>
@@ -3766,34 +3778,37 @@
         <v>111</v>
       </c>
       <c r="L221" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="222" spans="5:12">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="5:13">
       <c r="H222" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I222" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J222" s="8"/>
       <c r="K222" s="5" t="s">
         <v>111</v>
       </c>
       <c r="L222" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="223" spans="5:12">
+        <v>231</v>
+      </c>
+      <c r="M222" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="223" spans="5:13">
       <c r="G223" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I223" s="13"/>
       <c r="J223" s="13"/>
       <c r="K223" s="14"/>
       <c r="L223" s="14"/>
     </row>
-    <row r="224" spans="5:12">
+    <row r="224" spans="5:13">
       <c r="H224" s="1" t="s">
         <v>68</v>
       </c>
@@ -3807,7 +3822,7 @@
         <v>111</v>
       </c>
       <c r="L224" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="225" spans="6:13">
@@ -3824,7 +3839,10 @@
         <v>111</v>
       </c>
       <c r="L225" s="5" t="s">
-        <v>179</v>
+        <v>232</v>
+      </c>
+      <c r="M225" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="226" spans="6:13">
@@ -3841,7 +3859,7 @@
         <v>89</v>
       </c>
       <c r="L226" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="227" spans="6:13">
@@ -3939,7 +3957,7 @@
         <v>54</v>
       </c>
       <c r="I233" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J233" s="2" t="s">
         <v>20</v>
@@ -3948,10 +3966,10 @@
         <v>111</v>
       </c>
       <c r="L233" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="M233" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="234" spans="6:13">
@@ -4101,7 +4119,7 @@
     </row>
     <row r="259" spans="6:12">
       <c r="G259" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I259" s="2"/>
       <c r="J259" s="2"/>
@@ -4110,7 +4128,7 @@
     </row>
     <row r="260" spans="6:12">
       <c r="H260" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I260" s="2" t="s">
         <v>169</v>
@@ -4127,7 +4145,7 @@
     </row>
     <row r="261" spans="6:12">
       <c r="H261" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I261" s="2" t="s">
         <v>172</v>
@@ -4142,7 +4160,7 @@
     </row>
     <row r="262" spans="6:12">
       <c r="H262" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I262" s="2" t="s">
         <v>173</v>
@@ -4159,7 +4177,7 @@
     </row>
     <row r="263" spans="6:12">
       <c r="G263" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I263" s="2"/>
       <c r="J263" s="2"/>
@@ -4168,7 +4186,7 @@
     </row>
     <row r="264" spans="6:12">
       <c r="H264" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I264" s="2" t="s">
         <v>169</v>
@@ -4185,7 +4203,7 @@
     </row>
     <row r="265" spans="6:12">
       <c r="H265" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I265" s="2" t="s">
         <v>172</v>
@@ -4200,7 +4218,7 @@
     </row>
     <row r="266" spans="6:12">
       <c r="H266" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I266" s="2" t="s">
         <v>173</v>
@@ -4349,7 +4367,7 @@
         <v>111</v>
       </c>
       <c r="L275" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="276" spans="3:12">
@@ -4366,7 +4384,7 @@
         <v>89</v>
       </c>
       <c r="L276" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="278" spans="3:12">
@@ -4512,7 +4530,7 @@
         <v>32</v>
       </c>
       <c r="I305" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J305" s="2" t="s">
         <v>88</v>
@@ -4524,7 +4542,7 @@
         <v>112</v>
       </c>
       <c r="M305" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="306" spans="6:13">
@@ -4541,7 +4559,7 @@
         <v>111</v>
       </c>
       <c r="L306" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="307" spans="6:13">
@@ -4554,7 +4572,7 @@
         <v>32</v>
       </c>
       <c r="I308" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J308" s="2" t="s">
         <v>88</v>
@@ -4566,7 +4584,7 @@
         <v>114</v>
       </c>
       <c r="M308" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="309" spans="6:13">
@@ -4577,7 +4595,7 @@
         <v>115</v>
       </c>
       <c r="J309" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K309" s="5" t="s">
         <v>111</v>
@@ -4613,7 +4631,7 @@
         <v>89</v>
       </c>
       <c r="L311" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="312" spans="6:13">
@@ -4658,7 +4676,7 @@
         <v>89</v>
       </c>
       <c r="L314" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="315" spans="6:13">
@@ -4698,7 +4716,7 @@
         <v>149</v>
       </c>
       <c r="M317" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="318" spans="6:13">
@@ -4715,7 +4733,7 @@
         <v>111</v>
       </c>
       <c r="L318" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M318" s="23"/>
     </row>
@@ -4733,7 +4751,7 @@
         <v>111</v>
       </c>
       <c r="L319" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M319" s="23"/>
     </row>
@@ -4747,7 +4765,7 @@
         <v>32</v>
       </c>
       <c r="I321" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J321" s="2" t="s">
         <v>88</v>
@@ -4759,7 +4777,7 @@
         <v>120</v>
       </c>
       <c r="M321" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="322" spans="5:13">
@@ -4791,7 +4809,7 @@
         <v>89</v>
       </c>
       <c r="L323" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="324" spans="5:13">
@@ -4828,7 +4846,7 @@
         <v>89</v>
       </c>
       <c r="L326" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="327" spans="5:13">
@@ -4845,7 +4863,7 @@
         <v>89</v>
       </c>
       <c r="L327" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="328" spans="5:13">
@@ -4862,7 +4880,7 @@
         <v>89</v>
       </c>
       <c r="L328" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="329" spans="5:13">
@@ -4879,7 +4897,7 @@
         <v>111</v>
       </c>
       <c r="L329" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="330" spans="5:13">
@@ -4896,7 +4914,7 @@
         <v>111</v>
       </c>
       <c r="L330" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="331" spans="5:13">
@@ -4913,7 +4931,7 @@
         <v>111</v>
       </c>
       <c r="L331" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="332" spans="5:13">
@@ -4930,12 +4948,12 @@
         <v>111</v>
       </c>
       <c r="L332" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="333" spans="5:13">
       <c r="G333" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I333" s="13"/>
       <c r="J333" s="13"/>
@@ -4956,7 +4974,7 @@
         <v>111</v>
       </c>
       <c r="L334" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="335" spans="5:13">
@@ -4964,19 +4982,22 @@
         <v>69</v>
       </c>
       <c r="I335" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J335" s="8"/>
       <c r="K335" s="5" t="s">
         <v>111</v>
       </c>
       <c r="L335" s="5" t="s">
-        <v>185</v>
+        <v>231</v>
+      </c>
+      <c r="M335" s="1" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="336" spans="5:13">
       <c r="G336" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I336" s="13"/>
       <c r="J336" s="13"/>
@@ -4997,7 +5018,7 @@
         <v>111</v>
       </c>
       <c r="L337" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="338" spans="6:13">
@@ -5014,7 +5035,10 @@
         <v>111</v>
       </c>
       <c r="L338" s="5" t="s">
-        <v>179</v>
+        <v>232</v>
+      </c>
+      <c r="M338" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="339" spans="6:13">
@@ -5031,7 +5055,7 @@
         <v>89</v>
       </c>
       <c r="L339" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="340" spans="6:13">
@@ -5129,7 +5153,7 @@
         <v>54</v>
       </c>
       <c r="I346" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J346" s="2" t="s">
         <v>20</v>
@@ -5138,10 +5162,10 @@
         <v>111</v>
       </c>
       <c r="L346" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="M346" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="347" spans="6:13">
@@ -5291,7 +5315,7 @@
     </row>
     <row r="372" spans="6:12">
       <c r="G372" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I372" s="2"/>
       <c r="J372" s="2"/>
@@ -5300,7 +5324,7 @@
     </row>
     <row r="373" spans="6:12">
       <c r="H373" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I373" s="2" t="s">
         <v>169</v>
@@ -5317,7 +5341,7 @@
     </row>
     <row r="374" spans="6:12">
       <c r="H374" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I374" s="2" t="s">
         <v>172</v>
@@ -5332,7 +5356,7 @@
     </row>
     <row r="375" spans="6:12">
       <c r="H375" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I375" s="2" t="s">
         <v>173</v>
@@ -5349,7 +5373,7 @@
     </row>
     <row r="376" spans="6:12">
       <c r="G376" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I376" s="2"/>
       <c r="J376" s="2"/>
@@ -5358,7 +5382,7 @@
     </row>
     <row r="377" spans="6:12">
       <c r="H377" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I377" s="2" t="s">
         <v>169</v>
@@ -5375,7 +5399,7 @@
     </row>
     <row r="378" spans="6:12">
       <c r="H378" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I378" s="2" t="s">
         <v>172</v>
@@ -5390,7 +5414,7 @@
     </row>
     <row r="379" spans="6:12">
       <c r="H379" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I379" s="2" t="s">
         <v>173</v>
@@ -5539,7 +5563,7 @@
         <v>111</v>
       </c>
       <c r="L388" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="389" spans="3:12">
@@ -5556,7 +5580,7 @@
         <v>89</v>
       </c>
       <c r="L389" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="390" spans="3:12">
@@ -5567,10 +5591,10 @@
     </row>
     <row r="392" spans="3:12" ht="46" customHeight="1">
       <c r="C392" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I392" s="24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J392" s="24"/>
       <c r="K392" s="24"/>
@@ -5659,7 +5683,7 @@
         <v>89</v>
       </c>
       <c r="L398" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="399" spans="3:12">
@@ -5685,7 +5709,7 @@
         <v>101</v>
       </c>
       <c r="J400" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K400" s="3" t="s">
         <v>89</v>
@@ -5708,7 +5732,7 @@
         <v>89</v>
       </c>
       <c r="L401" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="402" spans="5:12">
@@ -5787,7 +5811,7 @@
         <v>107</v>
       </c>
       <c r="J406" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K406" s="3" t="s">
         <v>89</v>
@@ -5801,7 +5825,7 @@
         <v>27</v>
       </c>
       <c r="I407" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J407" s="2" t="s">
         <v>88</v>
@@ -5834,7 +5858,7 @@
         <v>109</v>
       </c>
       <c r="J409" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K409" s="3" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
time format and version update
</commit_message>
<xml_diff>
--- a/Documentation.xlsx
+++ b/Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinzimmermann/Github/refractive-JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319CC651-EF3F-3C47-BA30-6A85093769AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15138AD-5744-D145-BE9A-310ADCF555DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{97470A89-5A9D-474B-83A0-7CF02DF1D5C9}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{97470A89-5A9D-474B-83A0-7CF02DF1D5C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="237">
   <si>
     <t>{</t>
   </si>
@@ -824,7 +823,13 @@
     <t>This field is mandatory if a Vertical prism power is entered</t>
   </si>
   <si>
-    <t>jsonVersion:0.1.4,</t>
+    <t>jsonVersion:0.1.5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time (H:M:S) ISO 8601 UTC </t>
+  </si>
+  <si>
+    <t>15:45:10</t>
   </si>
 </sst>
 </file>
@@ -1305,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CFF79E-0D8B-AF4F-8800-07737C044728}">
   <dimension ref="A1:Q410"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A355" zoomScale="137" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1"/>
@@ -1621,7 +1626,7 @@
         <v>17</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>97</v>
+        <v>235</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>87</v>
@@ -1630,7 +1635,7 @@
         <v>83</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>151</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="5:13">
@@ -2302,73 +2307,73 @@
       </c>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="69" spans="6:13" outlineLevel="1">
       <c r="G69" s="1" t="s">
         <v>40</v>
       </c>
       <c r="K69" s="3"/>
     </row>
-    <row r="70" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="70" spans="6:13" outlineLevel="1">
       <c r="G70" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K70" s="3"/>
     </row>
-    <row r="71" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="71" spans="6:13" outlineLevel="1">
       <c r="G71" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K71" s="3"/>
     </row>
-    <row r="72" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="72" spans="6:13" outlineLevel="1">
       <c r="G72" s="1" t="s">
         <v>43</v>
       </c>
       <c r="K72" s="3"/>
     </row>
-    <row r="73" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="73" spans="6:13" outlineLevel="1">
       <c r="G73" s="1" t="s">
         <v>44</v>
       </c>
       <c r="K73" s="3"/>
     </row>
-    <row r="74" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="74" spans="6:13" outlineLevel="1">
       <c r="G74" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K74" s="3"/>
     </row>
-    <row r="75" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="75" spans="6:13" outlineLevel="1">
       <c r="G75" s="1" t="s">
         <v>46</v>
       </c>
       <c r="K75" s="3"/>
     </row>
-    <row r="76" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="76" spans="6:13" outlineLevel="1">
       <c r="G76" s="1" t="s">
         <v>47</v>
       </c>
       <c r="K76" s="3"/>
     </row>
-    <row r="77" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="77" spans="6:13" outlineLevel="1">
       <c r="G77" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K77" s="3"/>
     </row>
-    <row r="78" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="78" spans="6:13" outlineLevel="1">
       <c r="G78" s="1" t="s">
         <v>49</v>
       </c>
       <c r="K78" s="3"/>
     </row>
-    <row r="79" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="79" spans="6:13" outlineLevel="1">
       <c r="G79" s="1" t="s">
         <v>50</v>
       </c>
       <c r="K79" s="3"/>
     </row>
-    <row r="80" spans="6:13" collapsed="1">
+    <row r="80" spans="6:13">
       <c r="F80" s="1" t="s">
         <v>52</v>
       </c>
@@ -2526,117 +2531,117 @@
         <v>146</v>
       </c>
     </row>
-    <row r="92" spans="3:13" hidden="1" outlineLevel="1">
+    <row r="92" spans="3:13" outlineLevel="1">
       <c r="E92" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="3:13" hidden="1" outlineLevel="1">
+    <row r="93" spans="3:13" outlineLevel="1">
       <c r="E93" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="3:13" hidden="1" outlineLevel="1">
+    <row r="94" spans="3:13" outlineLevel="1">
       <c r="E94" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="3:13" hidden="1" outlineLevel="1">
+    <row r="95" spans="3:13" outlineLevel="1">
       <c r="E95" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="3:13" hidden="1" outlineLevel="1">
+    <row r="96" spans="3:13" outlineLevel="1">
       <c r="E96" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="97" spans="5:6" outlineLevel="1">
       <c r="E97" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="98" spans="5:6" outlineLevel="1">
       <c r="E98" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="99" spans="5:6" outlineLevel="1">
       <c r="E99" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="100" spans="5:6" outlineLevel="1">
       <c r="E100" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="101" spans="5:6" outlineLevel="1">
       <c r="E101" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="102" spans="5:6" outlineLevel="1">
       <c r="E102" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="103" spans="5:6" outlineLevel="1">
       <c r="F103" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="104" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="104" spans="5:6" outlineLevel="1">
       <c r="F104" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="105" spans="5:6" outlineLevel="1">
       <c r="F105" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="106" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="106" spans="5:6" outlineLevel="1">
       <c r="F106" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="107" spans="5:6" outlineLevel="1">
       <c r="F107" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="108" spans="5:6" outlineLevel="1">
       <c r="F108" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="109" spans="5:6" outlineLevel="1">
       <c r="F109" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="110" spans="5:6" outlineLevel="1">
       <c r="F110" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="111" spans="5:6" outlineLevel="1">
       <c r="E111" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="5:6" hidden="1" outlineLevel="1">
+    <row r="112" spans="5:6" outlineLevel="1">
       <c r="F112" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="113" spans="4:13" outlineLevel="1">
       <c r="F113" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="114" spans="4:13" collapsed="1">
+    <row r="114" spans="4:13">
       <c r="D114" s="1" t="s">
         <v>29</v>
       </c>
@@ -3055,7 +3060,7 @@
       <c r="K143" s="14"/>
       <c r="L143" s="14"/>
     </row>
-    <row r="144" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="144" spans="6:13" outlineLevel="1">
       <c r="G144" s="1" t="s">
         <v>40</v>
       </c>
@@ -3072,87 +3077,87 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="145" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="145" spans="7:8" outlineLevel="1">
       <c r="G145" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="146" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="146" spans="7:8" outlineLevel="1">
       <c r="G146" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="147" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="147" spans="7:8" outlineLevel="1">
       <c r="G147" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="148" spans="7:8" outlineLevel="1">
       <c r="G148" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="149" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="149" spans="7:8" outlineLevel="1">
       <c r="G149" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="150" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="150" spans="7:8" outlineLevel="1">
       <c r="G150" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="151" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="151" spans="7:8" outlineLevel="1">
       <c r="G151" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="152" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="152" spans="7:8" outlineLevel="1">
       <c r="G152" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="153" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="153" spans="7:8" outlineLevel="1">
       <c r="G153" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="154" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="154" spans="7:8" outlineLevel="1">
       <c r="G154" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="155" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="155" spans="7:8" outlineLevel="1">
       <c r="H155" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="156" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="156" spans="7:8" outlineLevel="1">
       <c r="H156" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="157" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="157" spans="7:8" outlineLevel="1">
       <c r="G157" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="158" spans="7:8" outlineLevel="1">
       <c r="H158" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="159" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="159" spans="7:8" outlineLevel="1">
       <c r="H159" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="160" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="160" spans="7:8" outlineLevel="1">
       <c r="G160" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="161" spans="3:12" collapsed="1">
+    <row r="161" spans="3:12">
       <c r="F161" s="1" t="s">
         <v>52</v>
       </c>
@@ -3204,117 +3209,117 @@
         <v>146</v>
       </c>
     </row>
-    <row r="167" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="167" spans="3:12" outlineLevel="1">
       <c r="E167" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="168" spans="3:12" outlineLevel="1">
       <c r="E168" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="169" spans="3:12" outlineLevel="1">
       <c r="E169" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="170" spans="3:12" outlineLevel="1">
       <c r="E170" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="171" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="171" spans="3:12" outlineLevel="1">
       <c r="E171" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="172" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="172" spans="3:12" outlineLevel="1">
       <c r="E172" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="173" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="173" spans="3:12" outlineLevel="1">
       <c r="E173" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="174" spans="3:12" outlineLevel="1">
       <c r="E174" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="175" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="175" spans="3:12" outlineLevel="1">
       <c r="E175" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="176" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="176" spans="3:12" outlineLevel="1">
       <c r="E176" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="177" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="177" spans="4:13" outlineLevel="1">
       <c r="E177" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="178" spans="4:13" outlineLevel="1">
       <c r="F178" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="179" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="179" spans="4:13" outlineLevel="1">
       <c r="F179" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="180" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="180" spans="4:13" outlineLevel="1">
       <c r="F180" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="181" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="181" spans="4:13" outlineLevel="1">
       <c r="F181" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="182" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="182" spans="4:13" outlineLevel="1">
       <c r="F182" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="183" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="183" spans="4:13" outlineLevel="1">
       <c r="F183" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="184" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="184" spans="4:13" outlineLevel="1">
       <c r="F184" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="185" spans="4:13" outlineLevel="1">
       <c r="F185" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="186" spans="4:13" outlineLevel="1">
       <c r="E186" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="187" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="187" spans="4:13" outlineLevel="1">
       <c r="F187" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="4:13" hidden="1" outlineLevel="1">
+    <row r="188" spans="4:13" outlineLevel="1">
       <c r="F188" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="189" spans="4:13" collapsed="1">
+    <row r="189" spans="4:13">
       <c r="D189" s="1" t="s">
         <v>29</v>
       </c>
@@ -3987,122 +3992,122 @@
       </c>
       <c r="L234" s="2"/>
     </row>
-    <row r="235" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="235" spans="6:13" outlineLevel="1">
       <c r="G235" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="236" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="236" spans="6:13" outlineLevel="1">
       <c r="G236" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="237" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="237" spans="6:13" outlineLevel="1">
       <c r="G237" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="238" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="238" spans="6:13" outlineLevel="1">
       <c r="G238" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="239" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="239" spans="6:13" outlineLevel="1">
       <c r="G239" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="240" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="240" spans="6:13" outlineLevel="1">
       <c r="G240" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="241" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="241" spans="7:8" outlineLevel="1">
       <c r="G241" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="242" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="242" spans="7:8" outlineLevel="1">
       <c r="G242" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="243" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="243" spans="7:8" outlineLevel="1">
       <c r="G243" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="244" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="244" spans="7:8" outlineLevel="1">
       <c r="G244" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="245" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="245" spans="7:8" outlineLevel="1">
       <c r="H245" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="246" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="246" spans="7:8" outlineLevel="1">
       <c r="H246" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="247" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="247" spans="7:8" outlineLevel="1">
       <c r="G247" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="248" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="248" spans="7:8" outlineLevel="1">
       <c r="H248" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="249" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="249" spans="7:8" outlineLevel="1">
       <c r="H249" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="250" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="250" spans="7:8" outlineLevel="1">
       <c r="G250" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="251" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="251" spans="7:8" outlineLevel="1">
       <c r="G251" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="252" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="252" spans="7:8" outlineLevel="1">
       <c r="G252" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="253" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="253" spans="7:8" outlineLevel="1">
       <c r="G253" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="254" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="254" spans="7:8" outlineLevel="1">
       <c r="G254" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="255" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="255" spans="7:8" outlineLevel="1">
       <c r="G255" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="256" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="256" spans="7:8" outlineLevel="1">
       <c r="G256" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="257" spans="6:12" hidden="1" outlineLevel="1">
+    <row r="257" spans="6:12" outlineLevel="1">
       <c r="G257" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="258" spans="6:12" collapsed="1">
+    <row r="258" spans="6:12">
       <c r="F258" s="1" t="s">
         <v>52</v>
       </c>
@@ -4400,117 +4405,117 @@
         <v>146</v>
       </c>
     </row>
-    <row r="280" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="280" spans="3:12" outlineLevel="1">
       <c r="E280" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="281" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="281" spans="3:12" outlineLevel="1">
       <c r="E281" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="282" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="282" spans="3:12" outlineLevel="1">
       <c r="E282" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="283" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="283" spans="3:12" outlineLevel="1">
       <c r="E283" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="284" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="284" spans="3:12" outlineLevel="1">
       <c r="E284" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="285" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="285" spans="3:12" outlineLevel="1">
       <c r="E285" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="286" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="286" spans="3:12" outlineLevel="1">
       <c r="E286" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="287" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="287" spans="3:12" outlineLevel="1">
       <c r="E287" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="288" spans="3:12" hidden="1" outlineLevel="1">
+    <row r="288" spans="3:12" outlineLevel="1">
       <c r="E288" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="289" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="289" spans="4:6" outlineLevel="1">
       <c r="E289" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="290" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="290" spans="4:6" outlineLevel="1">
       <c r="E290" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="291" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="291" spans="4:6" outlineLevel="1">
       <c r="F291" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="292" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="292" spans="4:6" outlineLevel="1">
       <c r="F292" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="293" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="293" spans="4:6" outlineLevel="1">
       <c r="F293" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="294" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="294" spans="4:6" outlineLevel="1">
       <c r="F294" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="295" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="295" spans="4:6" outlineLevel="1">
       <c r="F295" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="296" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="296" spans="4:6" outlineLevel="1">
       <c r="F296" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="297" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="297" spans="4:6" outlineLevel="1">
       <c r="F297" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="298" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="298" spans="4:6" outlineLevel="1">
       <c r="F298" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="299" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="299" spans="4:6" outlineLevel="1">
       <c r="E299" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="300" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="300" spans="4:6" outlineLevel="1">
       <c r="F300" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="301" spans="4:6" hidden="1" outlineLevel="1">
+    <row r="301" spans="4:6" outlineLevel="1">
       <c r="F301" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="302" spans="4:6" collapsed="1">
+    <row r="302" spans="4:6">
       <c r="D302" s="1" t="s">
         <v>29</v>
       </c>
@@ -5183,122 +5188,122 @@
       </c>
       <c r="L347" s="2"/>
     </row>
-    <row r="348" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="348" spans="6:13" outlineLevel="1">
       <c r="G348" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="349" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="349" spans="6:13" outlineLevel="1">
       <c r="G349" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="350" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="350" spans="6:13" outlineLevel="1">
       <c r="G350" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="351" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="351" spans="6:13" outlineLevel="1">
       <c r="G351" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="352" spans="6:13" hidden="1" outlineLevel="1">
+    <row r="352" spans="6:13" outlineLevel="1">
       <c r="G352" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="353" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="353" spans="7:8" outlineLevel="1">
       <c r="G353" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="354" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="354" spans="7:8" outlineLevel="1">
       <c r="G354" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="355" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="355" spans="7:8" outlineLevel="1">
       <c r="G355" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="356" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="356" spans="7:8" outlineLevel="1">
       <c r="G356" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="357" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="357" spans="7:8" outlineLevel="1">
       <c r="G357" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="358" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="358" spans="7:8" outlineLevel="1">
       <c r="H358" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="359" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="359" spans="7:8" outlineLevel="1">
       <c r="H359" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="360" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="360" spans="7:8" outlineLevel="1">
       <c r="G360" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="361" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="361" spans="7:8" outlineLevel="1">
       <c r="H361" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="362" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="362" spans="7:8" outlineLevel="1">
       <c r="H362" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="363" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="363" spans="7:8" outlineLevel="1">
       <c r="G363" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="364" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="364" spans="7:8" outlineLevel="1">
       <c r="G364" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="365" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="365" spans="7:8" outlineLevel="1">
       <c r="G365" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="366" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="366" spans="7:8" outlineLevel="1">
       <c r="G366" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="367" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="367" spans="7:8" outlineLevel="1">
       <c r="G367" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="368" spans="7:8" hidden="1" outlineLevel="1">
+    <row r="368" spans="7:8" outlineLevel="1">
       <c r="G368" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="369" spans="6:12" hidden="1" outlineLevel="1">
+    <row r="369" spans="6:12" outlineLevel="1">
       <c r="G369" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="370" spans="6:12" hidden="1" outlineLevel="1">
+    <row r="370" spans="6:12" outlineLevel="1">
       <c r="G370" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="371" spans="6:12" collapsed="1">
+    <row r="371" spans="6:12">
       <c r="F371" s="1" t="s">
         <v>52</v>
       </c>

</xml_diff>